<commit_message>
Correction. Array now re-sets before each execution.
</commit_message>
<xml_diff>
--- a/FuntionTimes.xlsx
+++ b/FuntionTimes.xlsx
@@ -8,26 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnlittler/Desktop/Projects/Makers_Prep/Ruby_Challenges/Week_10_Challenges/sequence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FCA244-B9D9-B144-8C03-BE277011298C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76EC4A5-BE01-0644-A336-B0D8BC5B1288}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{9937CB98-5B21-A249-990E-3AC595101C89}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" activeTab="1" xr2:uid="{9937CB98-5B21-A249-990E-3AC595101C89}"/>
   </bookViews>
   <sheets>
     <sheet name="10,000" sheetId="1" r:id="rId1"/>
     <sheet name="1,000,000" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'1,000,000'!$A$3:$B$3</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'1,000,000'!$A$4:$B$4</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'1,000,000'!$A$5:$B$5</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'1,000,000'!$A$6:$B$6</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'1,000,000'!$C$1:$H$2</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'1,000,000'!$C$3:$H$3</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'1,000,000'!$C$4:$H$4</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'1,000,000'!$C$5:$H$5</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'1,000,000'!$C$6:$H$6</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -109,7 +98,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -118,6 +106,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -175,7 +164,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1800" b="1" u="sng"/>
-              <a:t>Algoritham Timing</a:t>
+              <a:t>Algoritham Timing (Nanoseconds)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -272,25 +261,25 @@
             <c:numRef>
               <c:f>'10,000'!$C$3:$H$3</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.20000000222353201</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.29999999969732</c:v>
+                  <c:v>99.999997473787502</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20000000222353201</c:v>
+                  <c:v>99.999997473787502</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.199999994947575</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.9999997473787502E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.9999997473787502E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -359,25 +348,25 @@
             <c:numRef>
               <c:f>'10,000'!$C$4:$H$4</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.3999999937368499</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3000000009778798</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.29999999667052</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.1999999999534303</c:v>
+                  <c:v>99.999997473787502</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.400000001653002</c:v>
+                  <c:v>100.000004749745</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.499999993829903</c:v>
+                  <c:v>100.000004749745</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -446,25 +435,25 @@
             <c:numRef>
               <c:f>'10,000'!$C$5:$H$5</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.9000000029336599</c:v>
+                  <c:v>99.999997473787502</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9999999947613105</c:v>
+                  <c:v>2000.00000040745</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1000000021304004</c:v>
+                  <c:v>1100.00000131549</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.9000000007217697</c:v>
+                  <c:v>700.000004144385</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.4999999991268</c:v>
+                  <c:v>899.99999909196004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.400000001653002</c:v>
+                  <c:v>899.99999909196004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -533,25 +522,25 @@
             <c:numRef>
               <c:f>'10,000'!$C$6:$H$6</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.39999999711290002</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.5</c:v>
+                  <c:v>3700.0000011175798</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.2999999984167</c:v>
+                  <c:v>7600.0000044586996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.699999997159399</c:v>
+                  <c:v>12499.999997089601</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31.499999997438799</c:v>
+                  <c:v>15400.0000038649</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>54.8000000054016</c:v>
+                  <c:v>19800.000001851</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -647,7 +636,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -780,6 +769,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="sng" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" u="sng" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Algoritham Timing (Nanoseconds)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -881,25 +900,25 @@
             <c:numRef>
               <c:f>'1,000,000'!$C$3:$H$3</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.29999999969732</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20000000222353201</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.300000006973277</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20000000222353201</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.20000000222353201</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.29999999969732</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -977,25 +996,25 @@
             <c:numRef>
               <c:f>'1,000,000'!$C$4:$H$4</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.19999999878928</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>141.79999999760099</c:v>
+                  <c:v>699.99999686842705</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>696.70000000041898</c:v>
+                  <c:v>1899.9999956577001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1601.6999999992499</c:v>
+                  <c:v>2499.9999950523402</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3570.5999999991</c:v>
+                  <c:v>4200.0000030384399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8209.9000000016495</c:v>
+                  <c:v>4099.9999982886902</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1073,25 +1092,25 @@
             <c:numRef>
               <c:f>'1,000,000'!$C$5:$H$5</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.40000000101281</c:v>
+                  <c:v>100.000004749745</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>195.20000000193201</c:v>
+                  <c:v>25000.000001455101</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>940.50000000424905</c:v>
+                  <c:v>48999.999999068597</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1865.5999999973501</c:v>
+                  <c:v>90799.999998125699</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4487.6000000003796</c:v>
+                  <c:v>105300.000002898</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7987.9000000000797</c:v>
+                  <c:v>136299.99999829999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1169,25 +1188,25 @@
             <c:numRef>
               <c:f>'1,000,000'!$C$6:$H$6</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.50000000192085203</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>669.300000001385</c:v>
+                  <c:v>409500.00000157102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1621.5000000011</c:v>
+                  <c:v>842299.99999661196</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3587.8999999986199</c:v>
+                  <c:v>1230599.9999953201</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6843.1000000055001</c:v>
+                  <c:v>1702199.9999997199</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11940.6999999991</c:v>
+                  <c:v>2021600.00000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1283,7 +1302,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2560,7 +2579,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -2895,7 +2914,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A6"/>
+      <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2906,132 +2925,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>10000</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>20000</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>30000</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>40000</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>50000</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
-        <v>0.20000000222353201</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.29999999969732</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.20000000222353201</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.199999994947575</v>
-      </c>
-      <c r="G3" s="1">
-        <v>9.9999997473787502E-2</v>
-      </c>
-      <c r="H3" s="1">
-        <v>9.9999997473787502E-2</v>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>99.999997473787502</v>
+      </c>
+      <c r="E3" s="5">
+        <v>99.999997473787502</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1">
-        <v>1.3999999937368499</v>
-      </c>
-      <c r="D4" s="1">
-        <v>6.3000000009778798</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3.29999999667052</v>
-      </c>
-      <c r="F4" s="1">
-        <v>7.1999999999534303</v>
-      </c>
-      <c r="G4" s="1">
-        <v>22.400000001653002</v>
-      </c>
-      <c r="H4" s="1">
-        <v>32.499999993829903</v>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>99.999997473787502</v>
+      </c>
+      <c r="G4" s="5">
+        <v>100.000004749745</v>
+      </c>
+      <c r="H4" s="5">
+        <v>100.000004749745</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
-        <v>1.9000000029336599</v>
-      </c>
-      <c r="D5" s="1">
-        <v>9.9999999947613105</v>
-      </c>
-      <c r="E5" s="1">
-        <v>5.1000000021304004</v>
-      </c>
-      <c r="F5" s="1">
-        <v>8.9000000007217697</v>
-      </c>
-      <c r="G5" s="1">
-        <v>22.4999999991268</v>
-      </c>
-      <c r="H5" s="1">
-        <v>22.400000001653002</v>
+      <c r="C5" s="5">
+        <v>99.999997473787502</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2000.00000040745</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1100.00000131549</v>
+      </c>
+      <c r="F5" s="5">
+        <v>700.000004144385</v>
+      </c>
+      <c r="G5" s="5">
+        <v>899.99999909196004</v>
+      </c>
+      <c r="H5" s="5">
+        <v>899.99999909196004</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1">
-        <v>0.39999999711290002</v>
-      </c>
-      <c r="D6" s="1">
-        <v>9.5</v>
-      </c>
-      <c r="E6" s="1">
-        <v>11.2999999984167</v>
-      </c>
-      <c r="F6" s="1">
-        <v>19.699999997159399</v>
-      </c>
-      <c r="G6" s="1">
-        <v>31.499999997438799</v>
-      </c>
-      <c r="H6" s="1">
-        <v>54.8000000054016</v>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3700.0000011175798</v>
+      </c>
+      <c r="E6" s="5">
+        <v>7600.0000044586996</v>
+      </c>
+      <c r="F6" s="5">
+        <v>12499.999997089601</v>
+      </c>
+      <c r="G6" s="5">
+        <v>15400.0000038649</v>
+      </c>
+      <c r="H6" s="5">
+        <v>19800.000001851</v>
       </c>
     </row>
   </sheetData>
@@ -3049,138 +3068,141 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N43" sqref="N43"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="18" max="18" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>1000000</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>2000000</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>3000000</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>4000000</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>5000000</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
-        <v>0.29999999969732</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.20000000222353201</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.300000006973277</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.20000000222353201</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.20000000222353201</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0.29999999969732</v>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1">
-        <v>1.19999999878928</v>
-      </c>
-      <c r="D4" s="1">
-        <v>141.79999999760099</v>
-      </c>
-      <c r="E4" s="1">
-        <v>696.70000000041898</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1601.6999999992499</v>
-      </c>
-      <c r="G4" s="1">
-        <v>3570.5999999991</v>
-      </c>
-      <c r="H4" s="1">
-        <v>8209.9000000016495</v>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>699.99999686842705</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1899.9999956577001</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2499.9999950523402</v>
+      </c>
+      <c r="G4" s="5">
+        <v>4200.0000030384399</v>
+      </c>
+      <c r="H4" s="5">
+        <v>4099.9999982886902</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
-        <v>1.40000000101281</v>
-      </c>
-      <c r="D5" s="1">
-        <v>195.20000000193201</v>
-      </c>
-      <c r="E5" s="1">
-        <v>940.50000000424905</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1865.5999999973501</v>
-      </c>
-      <c r="G5" s="1">
-        <v>4487.6000000003796</v>
-      </c>
-      <c r="H5" s="1">
-        <v>7987.9000000000797</v>
+      <c r="C5" s="5">
+        <v>100.000004749745</v>
+      </c>
+      <c r="D5" s="5">
+        <v>25000.000001455101</v>
+      </c>
+      <c r="E5" s="5">
+        <v>48999.999999068597</v>
+      </c>
+      <c r="F5" s="5">
+        <v>90799.999998125699</v>
+      </c>
+      <c r="G5" s="5">
+        <v>105300.000002898</v>
+      </c>
+      <c r="H5" s="5">
+        <v>136299.99999829999</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1">
-        <v>0.50000000192085203</v>
-      </c>
-      <c r="D6" s="1">
-        <v>669.300000001385</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1621.5000000011</v>
-      </c>
-      <c r="F6" s="1">
-        <v>3587.8999999986199</v>
-      </c>
-      <c r="G6" s="1">
-        <v>6843.1000000055001</v>
-      </c>
-      <c r="H6" s="1">
-        <v>11940.6999999991</v>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>409500.00000157102</v>
+      </c>
+      <c r="E6" s="5">
+        <v>842299.99999661196</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1230599.9999953201</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1702199.9999997199</v>
+      </c>
+      <c r="H6" s="5">
+        <v>2021600.00000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Algoritham to check an array for duplicates created within the framework. A function to synthesise the array has also been implemented.
</commit_message>
<xml_diff>
--- a/FuntionTimes.xlsx
+++ b/FuntionTimes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnlittler/Desktop/Projects/Makers_Prep/Ruby_Challenges/Week_10_Challenges/sequence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76EC4A5-BE01-0644-A336-B0D8BC5B1288}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDC09BA-D5C4-C04E-BCFB-E7DBFA181186}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" activeTab="1" xr2:uid="{9937CB98-5B21-A249-990E-3AC595101C89}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" xr2:uid="{9937CB98-5B21-A249-990E-3AC595101C89}"/>
   </bookViews>
   <sheets>
     <sheet name="10,000" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Reverse</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Function (time to complete)</t>
+  </si>
+  <si>
+    <t>CheckDuplicates</t>
   </si>
 </sst>
 </file>
@@ -549,6 +552,66 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-BF3E-2E49-9CB3-DC024A6C7C7D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'10,000'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CheckDuplicates</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'10,000'!$C$7:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>400.00000444706501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47900.000005029098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>169999.99999825301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>378899.99999606499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>682200.00001019798</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1054199.9999986701</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F0C6-EC4A-AF3B-140AA44E2FC7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1218,6 +1281,48 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1,000,000'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CheckDuplicates</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'1,000,000'!$C$7:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D5F7-D24A-97DA-FAF2027740EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2539,7 +2644,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
@@ -2579,8 +2684,8 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
@@ -2911,15 +3016,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DFF4342-DAFE-4F41-81ED-AEC72026D24D}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K1:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
     <col min="3" max="3" width="14.5" customWidth="1"/>
     <col min="4" max="8" width="12.83203125" customWidth="1"/>
   </cols>
@@ -3051,6 +3156,29 @@
       </c>
       <c r="H6" s="5">
         <v>19800.000001851</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5">
+        <v>400.00000444706501</v>
+      </c>
+      <c r="D7" s="5">
+        <v>47900.000005029098</v>
+      </c>
+      <c r="E7" s="5">
+        <v>169999.99999825301</v>
+      </c>
+      <c r="F7" s="5">
+        <v>378899.99999606499</v>
+      </c>
+      <c r="G7" s="5">
+        <v>682200.00001019798</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1054199.9999986701</v>
       </c>
     </row>
   </sheetData>
@@ -3065,14 +3193,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E79A092-EB17-0F45-B5EE-F33887CACCA1}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="18" max="18" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3205,6 +3334,17 @@
         <v>2021600.00000003</v>
       </c>
     </row>
+    <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:H1"/>

</xml_diff>

<commit_message>
Updated checkDuplicate function to improve efficiency.
</commit_message>
<xml_diff>
--- a/FuntionTimes.xlsx
+++ b/FuntionTimes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnlittler/Desktop/Projects/Makers_Prep/Ruby_Challenges/Week_10_Challenges/sequence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDC09BA-D5C4-C04E-BCFB-E7DBFA181186}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38818EE-EBFC-4E48-A6F2-59E1113E7113}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" xr2:uid="{9937CB98-5B21-A249-990E-3AC595101C89}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="1,000,000" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Reverse</t>
   </si>
@@ -47,6 +48,9 @@
   </si>
   <si>
     <t>CheckDuplicates</t>
+  </si>
+  <si>
+    <t>CheckDuplicates (refactored)</t>
   </si>
 </sst>
 </file>
@@ -103,13 +107,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -118,6 +122,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF914F5"/>
       <color rgb="FF6FFF5D"/>
     </mruColors>
   </colors>
@@ -612,6 +617,66 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F0C6-EC4A-AF3B-140AA44E2FC7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'10,000'!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CheckDuplicates (refactored)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="F914F5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'10,000'!$C$8:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>299.99999992469299</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2299.9999999910801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2499.9999999408801</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1499.9999999645199</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2799.9999999792599</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2099.9999999276001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A69D-4643-B10C-1988648DCAD6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1289,9 +1354,6 @@
               <c:f>'1,000,000'!$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>CheckDuplicates</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -2643,8 +2705,8 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
@@ -3016,28 +3078,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DFF4342-DAFE-4F41-81ED-AEC72026D24D}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K1:K19"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
     <col min="3" max="3" width="14.5" customWidth="1"/>
     <col min="4" max="8" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
@@ -3061,100 +3123,100 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>0</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>99.999997473787502</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>99.999997473787502</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
         <v>0</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="3">
         <v>0</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>0</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>99.999997473787502</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="3">
         <v>100.000004749745</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="3">
         <v>100.000004749745</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>99.999997473787502</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>2000.00000040745</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>1100.00000131549</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>700.000004144385</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="3">
         <v>899.99999909196004</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <v>899.99999909196004</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>0</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>3700.0000011175798</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>7600.0000044586996</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>12499.999997089601</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <v>15400.0000038649</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>19800.000001851</v>
       </c>
     </row>
@@ -3162,23 +3224,46 @@
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>400.00000444706501</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>47900.000005029098</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>169999.99999825301</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <v>378899.99999606499</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="3">
         <v>682200.00001019798</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="3">
         <v>1054199.9999986701</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
+        <v>299.99999992469299</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2299.9999999910801</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2499.9999999408801</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1499.9999999645199</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2799.9999999792599</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2099.9999999276001</v>
       </c>
     </row>
   </sheetData>
@@ -3196,7 +3281,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3206,14 +3291,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
@@ -3237,113 +3322,111 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>0</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>0</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>0</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
         <v>0</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="3">
         <v>0</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>699.99999686842705</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>1899.9999956577001</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>2499.9999950523402</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="3">
         <v>4200.0000030384399</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="3">
         <v>4099.9999982886902</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>100.000004749745</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>25000.000001455101</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>48999.999999068597</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>90799.999998125699</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="3">
         <v>105300.000002898</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <v>136299.99999829999</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>0</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>409500.00000157102</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>842299.99999661196</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>1230599.9999953201</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <v>1702199.9999997199</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>2021600.00000003</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Added my own methods for last and reverse, and timed them.
</commit_message>
<xml_diff>
--- a/FuntionTimes.xlsx
+++ b/FuntionTimes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnlittler/Desktop/Projects/Makers_Prep/Ruby_Challenges/Week_10_Challenges/sequence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38818EE-EBFC-4E48-A6F2-59E1113E7113}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66365487-EFE6-604E-9F60-97425C23E392}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" xr2:uid="{9937CB98-5B21-A249-990E-3AC595101C89}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{9937CB98-5B21-A249-990E-3AC595101C89}"/>
   </bookViews>
   <sheets>
     <sheet name="10,000" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>Reverse</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>CheckDuplicates (refactored)</t>
+  </si>
+  <si>
+    <t>myReverse</t>
   </si>
 </sst>
 </file>
@@ -391,7 +394,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'10,000'!$B$5</c:f>
+              <c:f>'10,000'!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -441,7 +444,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'10,000'!$C$5:$H$5</c:f>
+              <c:f>'10,000'!$C$6:$H$6</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -478,7 +481,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'10,000'!$B$6</c:f>
+              <c:f>'10,000'!$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -528,7 +531,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'10,000'!$C$6:$H$6</c:f>
+              <c:f>'10,000'!$C$7:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -565,7 +568,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'10,000'!$B$7</c:f>
+              <c:f>'10,000'!$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -588,7 +591,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'10,000'!$C$7:$H$7</c:f>
+              <c:f>'10,000'!$C$8:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -625,7 +628,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'10,000'!$B$8</c:f>
+              <c:f>'10,000'!$B$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -648,27 +651,27 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'10,000'!$C$8:$H$8</c:f>
+              <c:f>'10,000'!$C$9:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>299.99999992469299</c:v>
+                  <c:v>300.000000162981</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2299.9999999910801</c:v>
+                  <c:v>53199.999999836997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2499.9999999408801</c:v>
+                  <c:v>84499.999999941705</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1499.9999999645199</c:v>
+                  <c:v>122699.99999989499</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2799.9999999792599</c:v>
+                  <c:v>172300.00000016199</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2099.9999999276001</c:v>
+                  <c:v>234199.99999983699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -677,6 +680,68 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A69D-4643-B10C-1988648DCAD6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'10,000'!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>myReverse</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'10,000'!$C$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>99.999999292776906</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15199.999999822399</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53399.999999783096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11899.9999998777</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>203700.00000002599</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>342700.00000014901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A69D-4643-B10C-1988648DCAD6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1159,7 +1224,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1,000,000'!$A$5:$B$5</c:f>
+              <c:f>'1,000,000'!$A$6:$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1218,7 +1283,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1,000,000'!$C$5:$H$5</c:f>
+              <c:f>'1,000,000'!$C$6:$H$6</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1255,7 +1320,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1,000,000'!$A$6:$B$6</c:f>
+              <c:f>'1,000,000'!$A$7:$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1314,7 +1379,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1,000,000'!$C$6:$H$6</c:f>
+              <c:f>'1,000,000'!$C$7:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1351,9 +1416,12 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1,000,000'!$B$7</c:f>
+              <c:f>'1,000,000'!$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CheckDuplicates (refactored)</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1371,7 +1439,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'1,000,000'!$C$7:$H$7</c:f>
+              <c:f>'1,000,000'!$C$8:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1382,6 +1450,48 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D5F7-D24A-97DA-FAF2027740EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1,000,000'!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CheckDuplicates (refactored)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="F914F5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'1,000,000'!$C$8:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-91C4-F045-BD22-2A2209D8145C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2706,12 +2816,12 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2746,13 +2856,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3078,10 +3188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DFF4342-DAFE-4F41-81ED-AEC72026D24D}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="K18" sqref="K1:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3122,7 +3232,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -3175,101 +3285,127 @@
     <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3">
-        <v>99.999997473787502</v>
+        <v>99.999999292776906</v>
       </c>
       <c r="D5" s="3">
-        <v>2000.00000040745</v>
+        <v>15199.999999822399</v>
       </c>
       <c r="E5" s="3">
-        <v>1100.00000131549</v>
+        <v>53399.999999783096</v>
       </c>
       <c r="F5" s="3">
-        <v>700.000004144385</v>
+        <v>11899.9999998777</v>
       </c>
       <c r="G5" s="3">
-        <v>899.99999909196004</v>
+        <v>203700.00000002599</v>
       </c>
       <c r="H5" s="3">
-        <v>899.99999909196004</v>
+        <v>342700.00000014901</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3">
-        <v>0</v>
+        <v>99.999997473787502</v>
       </c>
       <c r="D6" s="3">
-        <v>3700.0000011175798</v>
+        <v>2000.00000040745</v>
       </c>
       <c r="E6" s="3">
-        <v>7600.0000044586996</v>
+        <v>1100.00000131549</v>
       </c>
       <c r="F6" s="3">
-        <v>12499.999997089601</v>
+        <v>700.000004144385</v>
       </c>
       <c r="G6" s="3">
-        <v>15400.0000038649</v>
+        <v>899.99999909196004</v>
       </c>
       <c r="H6" s="3">
-        <v>19800.000001851</v>
+        <v>899.99999909196004</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C7" s="3">
-        <v>400.00000444706501</v>
+        <v>0</v>
       </c>
       <c r="D7" s="3">
-        <v>47900.000005029098</v>
+        <v>3700.0000011175798</v>
       </c>
       <c r="E7" s="3">
-        <v>169999.99999825301</v>
+        <v>7600.0000044586996</v>
       </c>
       <c r="F7" s="3">
-        <v>378899.99999606499</v>
+        <v>12499.999997089601</v>
       </c>
       <c r="G7" s="3">
-        <v>682200.00001019798</v>
+        <v>15400.0000038649</v>
       </c>
       <c r="H7" s="3">
-        <v>1054199.9999986701</v>
+        <v>19800.000001851</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
       <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3">
+        <v>400.00000444706501</v>
+      </c>
+      <c r="D8" s="3">
+        <v>47900.000005029098</v>
+      </c>
+      <c r="E8" s="3">
+        <v>169999.99999825301</v>
+      </c>
+      <c r="F8" s="3">
+        <v>378899.99999606499</v>
+      </c>
+      <c r="G8" s="3">
+        <v>682200.00001019798</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1054199.9999986701</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3">
-        <v>299.99999992469299</v>
-      </c>
-      <c r="D8" s="3">
-        <v>2299.9999999910801</v>
-      </c>
-      <c r="E8" s="3">
-        <v>2499.9999999408801</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1499.9999999645199</v>
-      </c>
-      <c r="G8" s="3">
-        <v>2799.9999999792599</v>
-      </c>
-      <c r="H8" s="3">
-        <v>2099.9999999276001</v>
+      <c r="C9" s="3">
+        <v>300.000000162981</v>
+      </c>
+      <c r="D9" s="3">
+        <v>53199.999999836997</v>
+      </c>
+      <c r="E9" s="3">
+        <v>84499.999999941705</v>
+      </c>
+      <c r="F9" s="3">
+        <v>122699.99999989499</v>
+      </c>
+      <c r="G9" s="3">
+        <v>172300.00000016199</v>
+      </c>
+      <c r="H9" s="3">
+        <v>234199.99999983699</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A3:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3278,15 +3414,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E79A092-EB17-0F45-B5EE-F33887CACCA1}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" customWidth="1"/>
     <col min="18" max="18" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3321,7 +3457,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -3374,64 +3510,79 @@
     <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>100.000004749745</v>
-      </c>
-      <c r="D5" s="3">
-        <v>25000.000001455101</v>
-      </c>
-      <c r="E5" s="3">
-        <v>48999.999999068597</v>
-      </c>
-      <c r="F5" s="3">
-        <v>90799.999998125699</v>
-      </c>
-      <c r="G5" s="3">
-        <v>105300.000002898</v>
-      </c>
-      <c r="H5" s="3">
-        <v>136299.99999829999</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3">
-        <v>0</v>
+        <v>100.000004749745</v>
       </c>
       <c r="D6" s="3">
-        <v>409500.00000157102</v>
+        <v>25000.000001455101</v>
       </c>
       <c r="E6" s="3">
-        <v>842299.99999661196</v>
+        <v>48999.999999068597</v>
       </c>
       <c r="F6" s="3">
-        <v>1230599.9999953201</v>
+        <v>90799.999998125699</v>
       </c>
       <c r="G6" s="3">
-        <v>1702199.9999997199</v>
+        <v>105300.000002898</v>
       </c>
       <c r="H6" s="3">
-        <v>2021600.00000003</v>
+        <v>136299.99999829999</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>409500.00000157102</v>
+      </c>
+      <c r="E7" s="3">
+        <v>842299.99999661196</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1230599.9999953201</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1702199.9999997199</v>
+      </c>
+      <c r="H7" s="3">
+        <v>2021600.00000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A3:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Slight correction, removed an argument perameter.
</commit_message>
<xml_diff>
--- a/FuntionTimes.xlsx
+++ b/FuntionTimes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnlittler/Desktop/Projects/Makers_Prep/Ruby_Challenges/Week_10_Challenges/sequence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66365487-EFE6-604E-9F60-97425C23E392}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C08329-9A37-6540-BEEA-58146C1272FC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{9937CB98-5B21-A249-990E-3AC595101C89}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15980" xr2:uid="{9937CB98-5B21-A249-990E-3AC595101C89}"/>
   </bookViews>
   <sheets>
     <sheet name="10,000" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Reverse</t>
   </si>
@@ -727,7 +727,7 @@
                   <c:v>53399.999999783096</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11899.9999998777</c:v>
+                  <c:v>115500</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>203700.00000002599</c:v>
@@ -1224,7 +1224,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1,000,000'!$A$6:$B$6</c:f>
+              <c:f>'1,000,000'!$A$5:$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1283,7 +1283,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1,000,000'!$C$6:$H$6</c:f>
+              <c:f>'1,000,000'!$C$5:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1320,7 +1320,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1,000,000'!$A$7:$B$7</c:f>
+              <c:f>'1,000,000'!$A$6:$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1379,7 +1379,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1,000,000'!$C$7:$H$7</c:f>
+              <c:f>'1,000,000'!$C$6:$H$6</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1416,11 +1416,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1,000,000'!$B$8</c:f>
+              <c:f>'1,000,000'!#REF!</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CheckDuplicates (refactored)</c:v>
+                  <c:v>#REF!</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1428,7 +1428,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="7030A0"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1439,10 +1439,13 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'1,000,000'!$C$8:$H$8</c:f>
+              <c:f>'1,000,000'!#REF!</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1458,11 +1461,11 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1,000,000'!$B$8</c:f>
+              <c:f>'1,000,000'!#REF!</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CheckDuplicates (refactored)</c:v>
+                  <c:v>#REF!</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1470,7 +1473,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="F914F5"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1481,10 +1484,13 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'1,000,000'!$C$8:$H$8</c:f>
+              <c:f>'1,000,000'!#REF!</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2856,13 +2862,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3190,8 +3196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DFF4342-DAFE-4F41-81ED-AEC72026D24D}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="K18" sqref="K1:K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3297,7 +3303,7 @@
         <v>53399.999999783096</v>
       </c>
       <c r="F5" s="3">
-        <v>11899.9999998777</v>
+        <v>115500</v>
       </c>
       <c r="G5" s="3">
         <v>203700.00000002599</v>
@@ -3414,10 +3420,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E79A092-EB17-0F45-B5EE-F33887CACCA1}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3510,79 +3516,55 @@
     <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>100.000004749745</v>
+      </c>
+      <c r="D5" s="3">
+        <v>25000.000001455101</v>
+      </c>
+      <c r="E5" s="3">
+        <v>48999.999999068597</v>
+      </c>
+      <c r="F5" s="3">
+        <v>90799.999998125699</v>
+      </c>
+      <c r="G5" s="3">
+        <v>105300.000002898</v>
+      </c>
+      <c r="H5" s="3">
+        <v>136299.99999829999</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="3">
-        <v>100.000004749745</v>
+        <v>0</v>
       </c>
       <c r="D6" s="3">
-        <v>25000.000001455101</v>
+        <v>409500.00000157102</v>
       </c>
       <c r="E6" s="3">
-        <v>48999.999999068597</v>
+        <v>842299.99999661196</v>
       </c>
       <c r="F6" s="3">
-        <v>90799.999998125699</v>
+        <v>1230599.9999953201</v>
       </c>
       <c r="G6" s="3">
-        <v>105300.000002898</v>
+        <v>1702199.9999997199</v>
       </c>
       <c r="H6" s="3">
-        <v>136299.99999829999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>409500.00000157102</v>
-      </c>
-      <c r="E7" s="3">
-        <v>842299.99999661196</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1230599.9999953201</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1702199.9999997199</v>
-      </c>
-      <c r="H7" s="3">
         <v>2021600.00000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A3:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>